<commit_message>
saving changes made on the thesis write-up as well as all the other files after the long break
</commit_message>
<xml_diff>
--- a/AUTHOR_THOUGHTS/ABC_PAPERS_READ.xlsx
+++ b/AUTHOR_THOUGHTS/ABC_PAPERS_READ.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FRED\Dropbox\github\masters_project\AUTHOR_THOUGHTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo T470\Dropbox\github\masters_project\AUTHOR_THOUGHTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545D7C0D-2327-4915-AB0E-DCB0D52B26AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">PAPER TITLE </t>
   </si>
@@ -499,12 +500,65 @@
 - - A tolerance that is large enough so that all simulated data are accepted will produce a replica of the prior distribution</t>
     </r>
   </si>
+  <si>
+    <t>Bayesian calibration of computer models</t>
+  </si>
+  <si>
+    <t>M. C. Kennedy</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">** various sciences use mathematical models to describe processes that would otherwise be very difficult to analyze.
+** these models are often implemeted in computer codes
+** often, the model is highly complex and the resulting computer code is large and computationally expensive.
+** mathematical models are usually generic in nature.
+** However, in order to use them to make predictions in a specific setting and context, it is necessary to first calibrate the model by using data observed from the particular setting or context.
+** where there are no observed data, experiments can be performed to obtain observationl data
+** It is not possible to obtain the rates(parameters) themselves
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">** The observational data then are certain outputs of the model
+** calibration is the activity of adjusting the unknown rate parameters untill the outputs of the model fit as closely as possible to the observed data
+** these parameters are considered as estimates and the model is then used to make predictions concening the behavior of the process in a particular context. 
+** The reality about the parameter estimates is that they were not known and are only estimates
+** residual uncertainty about the parameters should be recognized in subsequent predictions from the model.
+** in particular, tere are several sources of uncertainty in the use of computer codes besides the uncertainty of parameter estimates  
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>** the Bayesian method here is built on the general bayesian approach to inference about unknown functions</t>
+    </r>
+  </si>
+  <si>
+    <t>Menzies 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Bayesian methods provide powerful tools for model calibration
+</t>
+  </si>
+  <si>
+    <t>Bayesian methods for calibrating Health policy models</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="31" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -721,6 +775,12 @@
     <font>
       <sz val="12"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1115,22 +1175,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="69.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.26953125" customWidth="1"/>
+    <col min="3" max="3" width="69.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1204,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1158,7 +1218,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1172,7 +1232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -1186,8 +1246,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="3"/>
+    <row r="5" spans="1:4" ht="333.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>